<commit_message>
fixing some features and bugs + optimisation
</commit_message>
<xml_diff>
--- a/php/excel/imprimantes_data.xlsx
+++ b/php/excel/imprimantes_data.xlsx
@@ -15,11 +15,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="18">
   <si>
     <t>ID</t>
   </si>
   <si>
+    <t>Modele</t>
+  </si>
+  <si>
     <t>Marque</t>
   </si>
   <si>
@@ -32,46 +35,40 @@
     <t>Stock</t>
   </si>
   <si>
-    <t>HP LaserJet Pro MFP</t>
+    <t>Epson EcoTank</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hp </t>
+  </si>
+  <si>
+    <t>168.192.102.28</t>
+  </si>
+  <si>
+    <t>exports</t>
+  </si>
+  <si>
+    <t>Epson laser 18</t>
   </si>
   <si>
     <t>hp</t>
   </si>
   <si>
+    <t>168.12.1.10</t>
+  </si>
+  <si>
     <t>achates</t>
   </si>
   <si>
-    <t>Epson EcoTank</t>
-  </si>
-  <si>
-    <t>168.192.102.28</t>
-  </si>
-  <si>
-    <t>production</t>
-  </si>
-  <si>
-    <t>Ricoh SP C</t>
+    <t>canon i-sensys lbp12x</t>
   </si>
   <si>
     <t>canon</t>
   </si>
   <si>
-    <t>168.12.1.10</t>
-  </si>
-  <si>
-    <t>Dell ColorSmart</t>
-  </si>
-  <si>
-    <t>informatique</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>f</t>
-  </si>
-  <si>
-    <t>1.3.2.3</t>
+    <t>168.12.10.5</t>
+  </si>
+  <si>
+    <t>productione</t>
   </si>
 </sst>
 </file>
@@ -411,10 +408,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="F6" sqref="A1"/>
+      <selection activeCell="F4" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -424,119 +421,79 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2">
-        <v>45</v>
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F2">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3">
         <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3">
-        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4">
-        <v>48</v>
+        <v>85</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4">
         <v>7</v>
-      </c>
-      <c r="F4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5">
-        <v>52</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5">
-        <v>52</v>
-      </c>
-      <c r="E5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6">
-        <v>77</v>
-      </c>
-      <c r="B6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>